<commit_message>
added new sheet for watermover parameters
</commit_message>
<xml_diff>
--- a/Example input/CO2_Respiration_CaseStudy1/CaseStudy1.xlsx
+++ b/Example input/CO2_Respiration_CaseStudy1/CaseStudy1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B19DF60-CBD0-411F-9BD3-290B2DD3EDA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034F3C78-159A-4B45-A223-BA1CB7B5141A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21570" yWindow="1995" windowWidth="17250" windowHeight="11820" tabRatio="626" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31470" yWindow="3990" windowWidth="17250" windowHeight="8910" tabRatio="626" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="16" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Weather" sheetId="7" r:id="rId16"/>
     <sheet name="MulchDecomp" sheetId="19" r:id="rId17"/>
     <sheet name="MulchGeo" sheetId="20" r:id="rId18"/>
+    <sheet name="WaterMovParam" sheetId="23" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Soil!$A$1:$A$1</definedName>
@@ -38,6 +39,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="10" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="18" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Soil">Soil!$A$1:$AT$1</definedName>
     <definedName name="Time">Time!$A$1:$K$1</definedName>
@@ -169,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2980" uniqueCount="480">
   <si>
     <t>Date</t>
   </si>
@@ -1574,6 +1576,42 @@
   <si>
     <t>N2O(ppm)</t>
   </si>
+  <si>
+    <t>WaterMovParam</t>
+  </si>
+  <si>
+    <t>WaterMovDefault</t>
+  </si>
+  <si>
+    <t>MaxIt</t>
+  </si>
+  <si>
+    <t>TolTh</t>
+  </si>
+  <si>
+    <t>TolH</t>
+  </si>
+  <si>
+    <t>hCritA</t>
+  </si>
+  <si>
+    <t>hCritS</t>
+  </si>
+  <si>
+    <t>DtMx</t>
+  </si>
+  <si>
+    <t>htab1</t>
+  </si>
+  <si>
+    <t>htabN</t>
+  </si>
+  <si>
+    <t>EPSI.Heat</t>
+  </si>
+  <si>
+    <t>EPSI.Solute</t>
+  </si>
 </sst>
 </file>
 
@@ -2167,12 +2205,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y88"/>
+  <dimension ref="A1:Z88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="S54" sqref="S54:S88"/>
+      <selection pane="bottomLeft" activeCell="V54" sqref="V54:V88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2195,10 +2233,10 @@
     <col min="17" max="17" width="24.6640625" customWidth="1"/>
     <col min="18" max="19" width="24.88671875" customWidth="1"/>
     <col min="20" max="20" width="16.109375" customWidth="1"/>
-    <col min="21" max="21" width="15.88671875" customWidth="1"/>
+    <col min="21" max="22" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2263,16 +2301,19 @@
         <v>228</v>
       </c>
       <c r="V1" t="s">
+        <v>468</v>
+      </c>
+      <c r="W1" t="s">
         <v>150</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>153</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>304</v>
       </c>
@@ -2340,17 +2381,20 @@
       <c r="U2" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V2" s="37" t="s">
+      <c r="V2" t="s">
+        <v>469</v>
+      </c>
+      <c r="W2" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X2" s="34" t="s">
+      <c r="Y2" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="Y2" s="32">
+      <c r="Z2" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>305</v>
       </c>
@@ -2419,18 +2463,21 @@
       <c r="U3" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V3" s="37" t="s">
+      <c r="V3" t="s">
+        <v>469</v>
+      </c>
+      <c r="W3" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X3" s="32" t="str">
-        <f>X2</f>
+      <c r="Y3" s="32" t="str">
+        <f>Y2</f>
         <v>R</v>
       </c>
-      <c r="Y3" s="32">
+      <c r="Z3" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>306</v>
       </c>
@@ -2499,18 +2546,21 @@
       <c r="U4" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V4" s="37" t="s">
+      <c r="V4" t="s">
+        <v>469</v>
+      </c>
+      <c r="W4" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X4" s="32" t="str">
-        <f t="shared" ref="X4:X67" si="5">X3</f>
+      <c r="Y4" s="32" t="str">
+        <f t="shared" ref="Y4:Y67" si="5">Y3</f>
         <v>R</v>
       </c>
-      <c r="Y4" s="32">
+      <c r="Z4" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>307</v>
       </c>
@@ -2579,18 +2629,21 @@
       <c r="U5" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V5" s="37" t="s">
+      <c r="V5" t="s">
+        <v>469</v>
+      </c>
+      <c r="W5" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X5" s="32" t="str">
+      <c r="Y5" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y5" s="32">
+      <c r="Z5" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>308</v>
       </c>
@@ -2659,18 +2712,21 @@
       <c r="U6" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V6" s="37" t="s">
+      <c r="V6" t="s">
+        <v>469</v>
+      </c>
+      <c r="W6" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X6" s="32" t="str">
+      <c r="Y6" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y6" s="32">
+      <c r="Z6" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="7" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>309</v>
       </c>
@@ -2739,18 +2795,21 @@
       <c r="U7" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V7" s="37" t="s">
+      <c r="V7" t="s">
+        <v>469</v>
+      </c>
+      <c r="W7" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X7" s="32" t="str">
+      <c r="Y7" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y7" s="32">
+      <c r="Z7" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="8" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>310</v>
       </c>
@@ -2819,18 +2878,21 @@
       <c r="U8" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V8" s="37" t="s">
+      <c r="V8" t="s">
+        <v>469</v>
+      </c>
+      <c r="W8" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X8" s="32" t="str">
+      <c r="Y8" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y8" s="32">
+      <c r="Z8" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="9" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
         <v>311</v>
       </c>
@@ -2899,18 +2961,21 @@
       <c r="U9" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V9" s="37" t="s">
+      <c r="V9" t="s">
+        <v>469</v>
+      </c>
+      <c r="W9" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X9" s="32" t="str">
+      <c r="Y9" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y9" s="32">
+      <c r="Z9" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>312</v>
       </c>
@@ -2979,18 +3044,21 @@
       <c r="U10" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V10" s="37" t="s">
+      <c r="V10" t="s">
+        <v>469</v>
+      </c>
+      <c r="W10" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X10" s="32" t="str">
+      <c r="Y10" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y10" s="32">
+      <c r="Z10" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
         <v>313</v>
       </c>
@@ -3059,18 +3127,21 @@
       <c r="U11" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V11" s="37" t="s">
+      <c r="V11" t="s">
+        <v>469</v>
+      </c>
+      <c r="W11" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X11" s="32" t="str">
+      <c r="Y11" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y11" s="32">
+      <c r="Z11" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="12" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="s">
         <v>314</v>
       </c>
@@ -3139,18 +3210,21 @@
       <c r="U12" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V12" s="37" t="s">
+      <c r="V12" t="s">
+        <v>469</v>
+      </c>
+      <c r="W12" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X12" s="32" t="str">
+      <c r="Y12" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y12" s="32">
+      <c r="Z12" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>315</v>
       </c>
@@ -3219,18 +3293,21 @@
       <c r="U13" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V13" s="37" t="s">
+      <c r="V13" t="s">
+        <v>469</v>
+      </c>
+      <c r="W13" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X13" s="32" t="str">
+      <c r="Y13" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y13" s="32">
+      <c r="Z13" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>316</v>
       </c>
@@ -3297,18 +3374,19 @@
       <c r="U14" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V14" s="37" t="s">
+      <c r="V14" s="37"/>
+      <c r="W14" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X14" s="32" t="str">
+      <c r="Y14" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y14" s="32">
+      <c r="Z14" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="15" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
         <v>317</v>
       </c>
@@ -3375,18 +3453,19 @@
       <c r="U15" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V15" s="37" t="s">
+      <c r="V15" s="37"/>
+      <c r="W15" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X15" s="32" t="str">
+      <c r="Y15" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y15" s="32">
+      <c r="Z15" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="16" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
         <v>318</v>
       </c>
@@ -3453,18 +3532,19 @@
       <c r="U16" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V16" s="37" t="s">
+      <c r="V16" s="37"/>
+      <c r="W16" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X16" s="32" t="str">
+      <c r="Y16" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y16" s="32">
+      <c r="Z16" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="17" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="35" t="s">
         <v>319</v>
       </c>
@@ -3532,18 +3612,19 @@
       <c r="U17" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V17" s="37" t="s">
+      <c r="V17" s="37"/>
+      <c r="W17" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X17" s="32" t="str">
+      <c r="Y17" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y17" s="32">
+      <c r="Z17" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="18" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="35" t="s">
         <v>320</v>
       </c>
@@ -3611,18 +3692,19 @@
       <c r="U18" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V18" s="37" t="s">
+      <c r="V18" s="37"/>
+      <c r="W18" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X18" s="32" t="str">
+      <c r="Y18" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y18" s="32">
+      <c r="Z18" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="35" t="s">
         <v>321</v>
       </c>
@@ -3690,18 +3772,19 @@
       <c r="U19" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V19" s="37" t="s">
+      <c r="V19" s="37"/>
+      <c r="W19" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X19" s="32" t="str">
+      <c r="Y19" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y19" s="32">
+      <c r="Z19" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="20" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="35" t="s">
         <v>322</v>
       </c>
@@ -3769,18 +3852,19 @@
       <c r="U20" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V20" s="37" t="s">
+      <c r="V20" s="37"/>
+      <c r="W20" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X20" s="32" t="str">
+      <c r="Y20" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y20" s="32">
+      <c r="Z20" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="21" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="35" t="s">
         <v>323</v>
       </c>
@@ -3848,18 +3932,19 @@
       <c r="U21" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V21" s="37" t="s">
+      <c r="V21" s="37"/>
+      <c r="W21" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X21" s="32" t="str">
+      <c r="Y21" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y21" s="32">
+      <c r="Z21" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="22" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="35" t="s">
         <v>324</v>
       </c>
@@ -3927,18 +4012,19 @@
       <c r="U22" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V22" s="37" t="s">
+      <c r="V22" s="37"/>
+      <c r="W22" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X22" s="32" t="str">
+      <c r="Y22" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y22" s="32">
+      <c r="Z22" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="23" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="35" t="s">
         <v>325</v>
       </c>
@@ -4006,18 +4092,19 @@
       <c r="U23" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V23" s="37" t="s">
+      <c r="V23" s="37"/>
+      <c r="W23" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X23" s="32" t="str">
+      <c r="Y23" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y23" s="32">
+      <c r="Z23" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="s">
         <v>326</v>
       </c>
@@ -4085,18 +4172,19 @@
       <c r="U24" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V24" s="37" t="s">
+      <c r="V24" s="37"/>
+      <c r="W24" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X24" s="32" t="str">
+      <c r="Y24" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y24" s="32">
+      <c r="Z24" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
         <v>327</v>
       </c>
@@ -4164,18 +4252,19 @@
       <c r="U25" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V25" s="37" t="s">
+      <c r="V25" s="37"/>
+      <c r="W25" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X25" s="32" t="str">
+      <c r="Y25" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y25" s="32">
+      <c r="Z25" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="26" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="35" t="s">
         <v>328</v>
       </c>
@@ -4243,18 +4332,19 @@
       <c r="U26" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V26" s="37" t="s">
+      <c r="V26" s="37"/>
+      <c r="W26" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X26" s="32" t="str">
+      <c r="Y26" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y26" s="32">
+      <c r="Z26" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="27" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="35" t="s">
         <v>329</v>
       </c>
@@ -4322,18 +4412,19 @@
       <c r="U27" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V27" s="37" t="s">
+      <c r="V27" s="37"/>
+      <c r="W27" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X27" s="32" t="str">
+      <c r="Y27" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y27" s="32">
+      <c r="Z27" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="28" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
         <v>330</v>
       </c>
@@ -4401,18 +4492,19 @@
       <c r="U28" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V28" s="37" t="s">
+      <c r="V28" s="37"/>
+      <c r="W28" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X28" s="32" t="str">
+      <c r="Y28" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y28" s="32">
+      <c r="Z28" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="29" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="35" t="s">
         <v>331</v>
       </c>
@@ -4480,18 +4572,19 @@
       <c r="U29" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V29" s="37" t="s">
+      <c r="V29" s="37"/>
+      <c r="W29" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X29" s="32" t="str">
+      <c r="Y29" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y29" s="32">
+      <c r="Z29" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="30" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="35" t="s">
         <v>332</v>
       </c>
@@ -4559,18 +4652,19 @@
       <c r="U30" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V30" s="37" t="s">
+      <c r="V30" s="37"/>
+      <c r="W30" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X30" s="32" t="str">
+      <c r="Y30" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y30" s="32">
+      <c r="Z30" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="31" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="35" t="s">
         <v>333</v>
       </c>
@@ -4638,18 +4732,19 @@
       <c r="U31" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V31" s="37" t="s">
+      <c r="V31" s="37"/>
+      <c r="W31" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X31" s="32" t="str">
+      <c r="Y31" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y31" s="32">
+      <c r="Z31" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
         <v>334</v>
       </c>
@@ -4717,18 +4812,19 @@
       <c r="U32" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V32" s="37" t="s">
+      <c r="V32" s="37"/>
+      <c r="W32" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X32" s="32" t="str">
+      <c r="Y32" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y32" s="32">
+      <c r="Z32" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="35" t="s">
         <v>335</v>
       </c>
@@ -4796,18 +4892,19 @@
       <c r="U33" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V33" s="37" t="s">
+      <c r="V33" s="37"/>
+      <c r="W33" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X33" s="32" t="str">
+      <c r="Y33" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y33" s="32">
+      <c r="Z33" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="34" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="35" t="s">
         <v>336</v>
       </c>
@@ -4875,18 +4972,19 @@
       <c r="U34" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V34" s="37" t="s">
+      <c r="V34" s="37"/>
+      <c r="W34" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X34" s="32" t="str">
+      <c r="Y34" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y34" s="32">
+      <c r="Z34" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="35" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>337</v>
       </c>
@@ -4954,18 +5052,19 @@
       <c r="U35" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V35" s="37" t="s">
+      <c r="V35" s="37"/>
+      <c r="W35" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X35" s="32" t="str">
+      <c r="Y35" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y35" s="32">
+      <c r="Z35" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>338</v>
       </c>
@@ -5033,18 +5132,19 @@
       <c r="U36" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V36" s="37" t="s">
+      <c r="V36" s="37"/>
+      <c r="W36" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X36" s="32" t="str">
+      <c r="Y36" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y36" s="32">
+      <c r="Z36" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="35" t="s">
         <v>339</v>
       </c>
@@ -5111,18 +5211,19 @@
       <c r="U37" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V37" s="37" t="s">
+      <c r="V37" s="37"/>
+      <c r="W37" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X37" s="32" t="str">
+      <c r="Y37" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y37" s="32">
+      <c r="Z37" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="35" t="s">
         <v>340</v>
       </c>
@@ -5189,18 +5290,19 @@
       <c r="U38" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V38" s="37" t="s">
+      <c r="V38" s="37"/>
+      <c r="W38" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X38" s="32" t="str">
+      <c r="Y38" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y38" s="32">
+      <c r="Z38" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="35" t="s">
         <v>341</v>
       </c>
@@ -5267,18 +5369,19 @@
       <c r="U39" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V39" s="37" t="s">
+      <c r="V39" s="37"/>
+      <c r="W39" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X39" s="32" t="str">
+      <c r="Y39" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y39" s="32">
+      <c r="Z39" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="40" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
         <v>342</v>
       </c>
@@ -5345,18 +5448,19 @@
       <c r="U40" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V40" s="37" t="s">
+      <c r="V40" s="37"/>
+      <c r="W40" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X40" s="32" t="str">
+      <c r="Y40" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y40" s="32">
+      <c r="Z40" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="41" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="35" t="s">
         <v>343</v>
       </c>
@@ -5423,18 +5527,19 @@
       <c r="U41" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V41" s="37" t="s">
+      <c r="V41" s="37"/>
+      <c r="W41" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X41" s="32" t="str">
+      <c r="Y41" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y41" s="32">
+      <c r="Z41" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="42" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="35" t="s">
         <v>344</v>
       </c>
@@ -5501,18 +5606,19 @@
       <c r="U42" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V42" s="37" t="s">
+      <c r="V42" s="37"/>
+      <c r="W42" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X42" s="32" t="str">
+      <c r="Y42" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y42" s="32">
+      <c r="Z42" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="43" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="35" t="s">
         <v>345</v>
       </c>
@@ -5579,18 +5685,19 @@
       <c r="U43" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V43" s="37" t="s">
+      <c r="V43" s="37"/>
+      <c r="W43" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X43" s="32" t="str">
+      <c r="Y43" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y43" s="32">
+      <c r="Z43" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="35" t="s">
         <v>346</v>
       </c>
@@ -5657,18 +5764,19 @@
       <c r="U44" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V44" s="37" t="s">
+      <c r="V44" s="37"/>
+      <c r="W44" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X44" s="32" t="str">
+      <c r="Y44" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y44" s="32">
+      <c r="Z44" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="35" t="s">
         <v>347</v>
       </c>
@@ -5735,18 +5843,19 @@
       <c r="U45" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V45" s="37" t="s">
+      <c r="V45" s="37"/>
+      <c r="W45" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X45" s="32" t="str">
+      <c r="Y45" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y45" s="32">
+      <c r="Z45" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="46" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="35" t="s">
         <v>348</v>
       </c>
@@ -5813,18 +5922,19 @@
       <c r="U46" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V46" s="37" t="s">
+      <c r="V46" s="37"/>
+      <c r="W46" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X46" s="32" t="str">
+      <c r="Y46" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y46" s="32">
+      <c r="Z46" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="47" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="35" t="s">
         <v>349</v>
       </c>
@@ -5891,18 +6001,19 @@
       <c r="U47" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V47" s="37" t="s">
+      <c r="V47" s="37"/>
+      <c r="W47" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X47" s="32" t="str">
+      <c r="Y47" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y47" s="32">
+      <c r="Z47" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="35" t="s">
         <v>350</v>
       </c>
@@ -5969,18 +6080,19 @@
       <c r="U48" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V48" s="37" t="s">
+      <c r="V48" s="37"/>
+      <c r="W48" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X48" s="32" t="str">
+      <c r="Y48" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y48" s="32">
+      <c r="Z48" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="49" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="35" t="s">
         <v>351</v>
       </c>
@@ -6047,18 +6159,19 @@
       <c r="U49" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V49" s="37" t="s">
+      <c r="V49" s="37"/>
+      <c r="W49" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X49" s="32" t="str">
+      <c r="Y49" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y49" s="32">
+      <c r="Z49" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="35" t="s">
         <v>352</v>
       </c>
@@ -6125,18 +6238,19 @@
       <c r="U50" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V50" s="37" t="s">
+      <c r="V50" s="37"/>
+      <c r="W50" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X50" s="32" t="str">
+      <c r="Y50" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y50" s="32">
+      <c r="Z50" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="35" t="s">
         <v>353</v>
       </c>
@@ -6203,18 +6317,19 @@
       <c r="U51" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V51" s="37" t="s">
+      <c r="V51" s="37"/>
+      <c r="W51" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X51" s="32" t="str">
+      <c r="Y51" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y51" s="32">
+      <c r="Z51" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="52" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="35" t="s">
         <v>354</v>
       </c>
@@ -6282,18 +6397,19 @@
       <c r="U52" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V52" s="37" t="s">
+      <c r="V52" s="37"/>
+      <c r="W52" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X52" s="32" t="str">
+      <c r="Y52" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y52" s="32">
+      <c r="Z52" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="35" t="s">
         <v>355</v>
       </c>
@@ -6361,18 +6477,19 @@
       <c r="U53" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V53" s="37" t="s">
+      <c r="V53" s="37"/>
+      <c r="W53" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X53" s="32" t="str">
+      <c r="Y53" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y53" s="32">
+      <c r="Z53" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="54" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="35" t="s">
         <v>356</v>
       </c>
@@ -6442,18 +6559,21 @@
       <c r="U54" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V54" s="37" t="s">
+      <c r="V54" t="s">
+        <v>469</v>
+      </c>
+      <c r="W54" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X54" s="32" t="str">
+      <c r="Y54" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y54" s="32">
+      <c r="Z54" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="55" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="35" t="s">
         <v>357</v>
       </c>
@@ -6523,18 +6643,21 @@
       <c r="U55" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V55" s="37" t="s">
+      <c r="V55" t="s">
+        <v>469</v>
+      </c>
+      <c r="W55" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X55" s="32" t="str">
+      <c r="Y55" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y55" s="32">
+      <c r="Z55" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="35" t="s">
         <v>358</v>
       </c>
@@ -6604,18 +6727,21 @@
       <c r="U56" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V56" s="37" t="s">
+      <c r="V56" t="s">
+        <v>469</v>
+      </c>
+      <c r="W56" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X56" s="32" t="str">
+      <c r="Y56" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y56" s="32">
+      <c r="Z56" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="57" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="35" t="s">
         <v>359</v>
       </c>
@@ -6685,18 +6811,21 @@
       <c r="U57" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V57" s="37" t="s">
+      <c r="V57" t="s">
+        <v>469</v>
+      </c>
+      <c r="W57" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X57" s="32" t="str">
+      <c r="Y57" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y57" s="32">
+      <c r="Z57" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="58" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="35" t="s">
         <v>360</v>
       </c>
@@ -6766,18 +6895,21 @@
       <c r="U58" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V58" s="37" t="s">
+      <c r="V58" t="s">
+        <v>469</v>
+      </c>
+      <c r="W58" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X58" s="32" t="str">
+      <c r="Y58" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y58" s="32">
+      <c r="Z58" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="59" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="35" t="s">
         <v>361</v>
       </c>
@@ -6847,18 +6979,21 @@
       <c r="U59" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V59" s="37" t="s">
+      <c r="V59" t="s">
+        <v>469</v>
+      </c>
+      <c r="W59" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X59" s="32" t="str">
+      <c r="Y59" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y59" s="32">
+      <c r="Z59" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="60" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="35" t="s">
         <v>362</v>
       </c>
@@ -6928,18 +7063,21 @@
       <c r="U60" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V60" s="37" t="s">
+      <c r="V60" t="s">
+        <v>469</v>
+      </c>
+      <c r="W60" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X60" s="32" t="str">
+      <c r="Y60" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y60" s="32">
+      <c r="Z60" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="61" spans="1:25" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="35" t="s">
         <v>363</v>
       </c>
@@ -7009,18 +7147,21 @@
       <c r="U61" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V61" s="37" t="s">
+      <c r="V61" t="s">
+        <v>469</v>
+      </c>
+      <c r="W61" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="X61" s="32" t="str">
+      <c r="Y61" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y61" s="32">
+      <c r="Z61" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="35" t="s">
         <v>395</v>
       </c>
@@ -7090,19 +7231,22 @@
       <c r="U62" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V62" s="37" t="s">
+      <c r="V62" t="s">
+        <v>469</v>
+      </c>
+      <c r="W62" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W62" s="32"/>
-      <c r="X62" s="32" t="str">
+      <c r="X62" s="32"/>
+      <c r="Y62" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y62" s="32">
+      <c r="Z62" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="63" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="35" t="s">
         <v>396</v>
       </c>
@@ -7172,19 +7316,22 @@
       <c r="U63" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V63" s="37" t="s">
+      <c r="V63" t="s">
+        <v>469</v>
+      </c>
+      <c r="W63" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W63" s="32"/>
-      <c r="X63" s="32" t="str">
+      <c r="X63" s="32"/>
+      <c r="Y63" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y63" s="32">
+      <c r="Z63" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="64" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="35" t="s">
         <v>397</v>
       </c>
@@ -7254,19 +7401,22 @@
       <c r="U64" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V64" s="37" t="s">
+      <c r="V64" t="s">
+        <v>469</v>
+      </c>
+      <c r="W64" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W64" s="32"/>
-      <c r="X64" s="32" t="str">
+      <c r="X64" s="32"/>
+      <c r="Y64" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y64" s="32">
+      <c r="Z64" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="65" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="35" t="s">
         <v>398</v>
       </c>
@@ -7336,19 +7486,22 @@
       <c r="U65" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V65" s="37" t="s">
+      <c r="V65" t="s">
+        <v>469</v>
+      </c>
+      <c r="W65" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W65" s="32"/>
-      <c r="X65" s="32" t="str">
+      <c r="X65" s="32"/>
+      <c r="Y65" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y65" s="32">
+      <c r="Z65" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="66" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="35" t="s">
         <v>399</v>
       </c>
@@ -7418,19 +7571,22 @@
       <c r="U66" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V66" s="37" t="s">
+      <c r="V66" t="s">
+        <v>469</v>
+      </c>
+      <c r="W66" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W66" s="32"/>
-      <c r="X66" s="32" t="str">
+      <c r="X66" s="32"/>
+      <c r="Y66" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y66" s="32">
+      <c r="Z66" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="67" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="35" t="s">
         <v>400</v>
       </c>
@@ -7500,19 +7656,22 @@
       <c r="U67" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V67" s="37" t="s">
+      <c r="V67" t="s">
+        <v>469</v>
+      </c>
+      <c r="W67" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W67" s="32"/>
-      <c r="X67" s="32" t="str">
+      <c r="X67" s="32"/>
+      <c r="Y67" s="32" t="str">
         <f t="shared" si="5"/>
         <v>R</v>
       </c>
-      <c r="Y67" s="32">
+      <c r="Z67" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="68" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="35" t="s">
         <v>401</v>
       </c>
@@ -7582,19 +7741,22 @@
       <c r="U68" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V68" s="37" t="s">
+      <c r="V68" t="s">
+        <v>469</v>
+      </c>
+      <c r="W68" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W68" s="32"/>
-      <c r="X68" s="32" t="str">
-        <f t="shared" ref="X68:X86" si="12">X67</f>
+      <c r="X68" s="32"/>
+      <c r="Y68" s="32" t="str">
+        <f t="shared" ref="Y68:Y86" si="12">Y67</f>
         <v>R</v>
       </c>
-      <c r="Y68" s="32">
+      <c r="Z68" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="69" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="35" t="s">
         <v>402</v>
       </c>
@@ -7664,19 +7826,22 @@
       <c r="U69" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V69" s="37" t="s">
+      <c r="V69" t="s">
+        <v>469</v>
+      </c>
+      <c r="W69" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W69" s="32"/>
-      <c r="X69" s="32" t="str">
+      <c r="X69" s="32"/>
+      <c r="Y69" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y69" s="32">
+      <c r="Z69" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="70" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="35" t="s">
         <v>403</v>
       </c>
@@ -7746,19 +7911,22 @@
       <c r="U70" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V70" s="37" t="s">
+      <c r="V70" t="s">
+        <v>469</v>
+      </c>
+      <c r="W70" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W70" s="32"/>
-      <c r="X70" s="32" t="str">
+      <c r="X70" s="32"/>
+      <c r="Y70" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y70" s="32">
+      <c r="Z70" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="71" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="35" t="s">
         <v>404</v>
       </c>
@@ -7828,19 +7996,22 @@
       <c r="U71" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V71" s="37" t="s">
+      <c r="V71" t="s">
+        <v>469</v>
+      </c>
+      <c r="W71" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W71" s="32"/>
-      <c r="X71" s="32" t="str">
+      <c r="X71" s="32"/>
+      <c r="Y71" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y71" s="32">
+      <c r="Z71" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="72" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="35" t="s">
         <v>405</v>
       </c>
@@ -7910,19 +8081,22 @@
       <c r="U72" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V72" s="37" t="s">
+      <c r="V72" t="s">
+        <v>469</v>
+      </c>
+      <c r="W72" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W72" s="32"/>
-      <c r="X72" s="32" t="str">
+      <c r="X72" s="32"/>
+      <c r="Y72" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y72" s="32">
+      <c r="Z72" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="73" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="35" t="s">
         <v>406</v>
       </c>
@@ -7992,19 +8166,22 @@
       <c r="U73" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V73" s="37" t="s">
+      <c r="V73" t="s">
+        <v>469</v>
+      </c>
+      <c r="W73" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W73" s="32"/>
-      <c r="X73" s="32" t="str">
+      <c r="X73" s="32"/>
+      <c r="Y73" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y73" s="32">
+      <c r="Z73" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="74" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="35" t="s">
         <v>407</v>
       </c>
@@ -8074,19 +8251,22 @@
       <c r="U74" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V74" s="37" t="s">
+      <c r="V74" t="s">
+        <v>469</v>
+      </c>
+      <c r="W74" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W74" s="32"/>
-      <c r="X74" s="32" t="str">
+      <c r="X74" s="32"/>
+      <c r="Y74" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y74" s="32">
+      <c r="Z74" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="75" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="35" t="s">
         <v>408</v>
       </c>
@@ -8156,19 +8336,22 @@
       <c r="U75" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V75" s="37" t="s">
+      <c r="V75" t="s">
+        <v>469</v>
+      </c>
+      <c r="W75" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W75" s="32"/>
-      <c r="X75" s="32" t="str">
+      <c r="X75" s="32"/>
+      <c r="Y75" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y75" s="32">
+      <c r="Z75" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="76" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="35" t="s">
         <v>409</v>
       </c>
@@ -8238,19 +8421,22 @@
       <c r="U76" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V76" s="37" t="s">
+      <c r="V76" t="s">
+        <v>469</v>
+      </c>
+      <c r="W76" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W76" s="32"/>
-      <c r="X76" s="32" t="str">
+      <c r="X76" s="32"/>
+      <c r="Y76" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y76" s="32">
+      <c r="Z76" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="77" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="35" t="s">
         <v>410</v>
       </c>
@@ -8320,19 +8506,22 @@
       <c r="U77" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V77" s="37" t="s">
+      <c r="V77" t="s">
+        <v>469</v>
+      </c>
+      <c r="W77" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W77" s="32"/>
-      <c r="X77" s="32" t="str">
+      <c r="X77" s="32"/>
+      <c r="Y77" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y77" s="32">
+      <c r="Z77" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="78" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="35" t="s">
         <v>411</v>
       </c>
@@ -8402,19 +8591,22 @@
       <c r="U78" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V78" s="37" t="s">
+      <c r="V78" t="s">
+        <v>469</v>
+      </c>
+      <c r="W78" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W78" s="32"/>
-      <c r="X78" s="32" t="str">
+      <c r="X78" s="32"/>
+      <c r="Y78" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y78" s="32">
+      <c r="Z78" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="79" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="35" t="s">
         <v>412</v>
       </c>
@@ -8484,19 +8676,22 @@
       <c r="U79" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V79" s="37" t="s">
+      <c r="V79" t="s">
+        <v>469</v>
+      </c>
+      <c r="W79" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W79" s="32"/>
-      <c r="X79" s="32" t="str">
+      <c r="X79" s="32"/>
+      <c r="Y79" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y79" s="32">
+      <c r="Z79" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="80" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="35" t="s">
         <v>413</v>
       </c>
@@ -8566,19 +8761,22 @@
       <c r="U80" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V80" s="37" t="s">
+      <c r="V80" t="s">
+        <v>469</v>
+      </c>
+      <c r="W80" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W80" s="32"/>
-      <c r="X80" s="32" t="str">
+      <c r="X80" s="32"/>
+      <c r="Y80" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y80" s="32">
+      <c r="Z80" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="81" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="35" t="s">
         <v>414</v>
       </c>
@@ -8648,19 +8846,22 @@
       <c r="U81" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V81" s="37" t="s">
+      <c r="V81" t="s">
+        <v>469</v>
+      </c>
+      <c r="W81" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W81" s="32"/>
-      <c r="X81" s="32" t="str">
+      <c r="X81" s="32"/>
+      <c r="Y81" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y81" s="32">
+      <c r="Z81" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="82" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="35" t="s">
         <v>415</v>
       </c>
@@ -8730,19 +8931,22 @@
       <c r="U82" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V82" s="37" t="s">
+      <c r="V82" t="s">
+        <v>469</v>
+      </c>
+      <c r="W82" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W82" s="32"/>
-      <c r="X82" s="32" t="str">
+      <c r="X82" s="32"/>
+      <c r="Y82" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y82" s="32">
+      <c r="Z82" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="83" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="35" t="s">
         <v>416</v>
       </c>
@@ -8812,19 +9016,22 @@
       <c r="U83" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V83" s="37" t="s">
+      <c r="V83" t="s">
+        <v>469</v>
+      </c>
+      <c r="W83" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W83" s="32"/>
-      <c r="X83" s="32" t="str">
+      <c r="X83" s="32"/>
+      <c r="Y83" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y83" s="32">
+      <c r="Z83" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="84" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="35" t="s">
         <v>417</v>
       </c>
@@ -8894,19 +9101,22 @@
       <c r="U84" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V84" s="37" t="s">
+      <c r="V84" t="s">
+        <v>469</v>
+      </c>
+      <c r="W84" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W84" s="32"/>
-      <c r="X84" s="32" t="str">
+      <c r="X84" s="32"/>
+      <c r="Y84" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y84" s="32">
+      <c r="Z84" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="85" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="35" t="s">
         <v>418</v>
       </c>
@@ -8976,19 +9186,22 @@
       <c r="U85" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V85" s="37" t="s">
+      <c r="V85" t="s">
+        <v>469</v>
+      </c>
+      <c r="W85" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W85" s="32"/>
-      <c r="X85" s="32" t="str">
+      <c r="X85" s="32"/>
+      <c r="Y85" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y85" s="32">
+      <c r="Z85" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="86" spans="1:25" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="35" t="s">
         <v>419</v>
       </c>
@@ -9058,19 +9271,22 @@
       <c r="U86" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="V86" s="37" t="s">
+      <c r="V86" t="s">
+        <v>469</v>
+      </c>
+      <c r="W86" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="W86" s="32"/>
-      <c r="X86" s="32" t="str">
+      <c r="X86" s="32"/>
+      <c r="Y86" s="32" t="str">
         <f t="shared" si="12"/>
         <v>R</v>
       </c>
-      <c r="Y86" s="32">
+      <c r="Z86" s="32">
         <v>2003</v>
       </c>
     </row>
-    <row r="87" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
         <v>296</v>
       </c>
@@ -9137,17 +9353,20 @@
       <c r="U87" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="V87" s="18" t="s">
+      <c r="V87" t="s">
+        <v>469</v>
+      </c>
+      <c r="W87" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="X87" s="18" t="s">
+      <c r="Y87" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="Y87">
+      <c r="Z87">
         <v>2004</v>
       </c>
     </row>
-    <row r="88" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
         <v>297</v>
       </c>
@@ -9216,13 +9435,16 @@
       <c r="U88" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="V88" s="18" t="s">
+      <c r="V88" t="s">
+        <v>469</v>
+      </c>
+      <c r="W88" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="X88" s="18" t="s">
+      <c r="Y88" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="Y88">
+      <c r="Z88">
         <v>2005</v>
       </c>
     </row>
@@ -14368,7 +14590,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AU233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q3" sqref="Q3:Q233"/>
     </sheetView>
@@ -52512,6 +52734,96 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF939A3-CFE1-4460-961B-EB2CAA71CA56}">
+  <sheetPr codeName="Sheet20"/>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E1" t="s">
+        <v>473</v>
+      </c>
+      <c r="F1" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1" t="s">
+        <v>475</v>
+      </c>
+      <c r="H1" t="s">
+        <v>476</v>
+      </c>
+      <c r="I1" t="s">
+        <v>477</v>
+      </c>
+      <c r="J1" t="s">
+        <v>478</v>
+      </c>
+      <c r="K1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>0.01</v>
+      </c>
+      <c r="D2">
+        <v>0.05</v>
+      </c>
+      <c r="E2" s="3">
+        <v>-100000</v>
+      </c>
+      <c r="F2" s="3">
+        <v>10000000000</v>
+      </c>
+      <c r="G2">
+        <v>0.02</v>
+      </c>
+      <c r="H2">
+        <v>1E-3</v>
+      </c>
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>0.5</v>
+      </c>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
@@ -67601,15 +67913,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086EABF47CD1113448A96A17F6C8D13F9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c68283fca48dae9b1add248de89d15c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a5f42ec3-4ee2-45fc-8d77-288bf2f0f986" xmlns:ns3="73fb875a-8af9-4255-b008-0995492d31cd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40d2b883f32ec076906f2da59f0ebb5f" ns2:_="" ns3:_="">
     <xsd:import namespace="a5f42ec3-4ee2-45fc-8d77-288bf2f0f986"/>
@@ -67798,15 +68101,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA6A39AF-B78F-46A4-B576-74869F9A9581}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDA73D10-6EB9-46B2-AEC6-EC67F487A9BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -67823,4 +68127,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA6A39AF-B78F-46A4-B576-74869F9A9581}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>